<commit_message>
ignore some file and add anew file
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\OneDrive\Desktop\git practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29B391D-19C8-4CC8-B5A4-B0780B885436}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AB1D96-732E-46BC-A361-4326BAE58D84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,8 +438,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>